<commit_message>
add results analysis for user study
</commit_message>
<xml_diff>
--- a/data/lab-study/survey-results.xlsx
+++ b/data/lab-study/survey-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\Documents\University\msciProject\tactihelm-l5project\data\lab-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223DCF78-AB7F-4A33-BA2D-F9AC560077BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69FECF3-3651-4B71-A8BB-293CD691630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="220">
   <si>
     <t>ID</t>
   </si>
@@ -721,24 +721,6 @@
   </si>
   <si>
     <t>Whilst rear vibrations were the hardest to detect, once detected they were the easiest to distinguish</t>
-  </si>
-  <si>
-    <t>I could sense the location of all, but I couldn't feel the middle one</t>
-  </si>
-  <si>
-    <t>&lt;5 metres</t>
-  </si>
-  <si>
-    <t>Helmet was too small so I couldn't feel the front or middle ones</t>
-  </si>
-  <si>
-    <t>Vibrations could be stronger/last longer when a car is iminent</t>
-  </si>
-  <si>
-    <t>Too small</t>
-  </si>
-  <si>
-    <t>More size options</t>
   </si>
 </sst>
 </file>
@@ -1315,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,6 +1495,24 @@
       <c r="J2" t="s">
         <v>58</v>
       </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" t="s">
+        <v>60</v>
+      </c>
       <c r="Q2" t="s">
         <v>59</v>
       </c>
@@ -4311,57 +4311,8 @@
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>45342.432581018496</v>
-      </c>
-      <c r="C21" s="1">
-        <v>45342.434143518498</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" t="s">
-        <v>220</v>
-      </c>
-      <c r="H21" t="s">
-        <v>221</v>
-      </c>
-      <c r="I21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS21" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV21" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX21">
-        <v>3</v>
-      </c>
-      <c r="AY21" t="s">
-        <v>224</v>
-      </c>
-      <c r="AZ21" t="s">
-        <v>225</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>